<commit_message>
complete level mockup w/ description of gameplay
</commit_message>
<xml_diff>
--- a/Art_Assets/Bryan/main level mockup.xlsx
+++ b/Art_Assets/Bryan/main level mockup.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="19">
   <si>
     <t>X</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t xml:space="preserve"> = AMMO</t>
+  </si>
+  <si>
+    <t>Player starts out in red hangar after his ship crashes. Since his ship is toast, he has to find a new one. He ventures down the green hallway.</t>
+  </si>
+  <si>
+    <t>You can see the final hangar (purple) with a brand-new ship. However, you unexpectedly fall down (where the x is) and have to navigate through the level to the stairs.</t>
+  </si>
+  <si>
+    <t>Debris may be added to close off areas as the level progresses. The ammo room is accessible throughout the game to refill as needed.</t>
+  </si>
+  <si>
+    <t>Standing bots simply hold their post and attack when they see you. Hallway bots patrol up and down the hallway and attack when they see you.</t>
+  </si>
+  <si>
+    <t>When you make it up the stairs into the final hangar with the new ship, you win.</t>
   </si>
 </sst>
 </file>
@@ -822,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CL37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -3743,7 +3758,10 @@
       <c r="CK32" s="15"/>
       <c r="CL32" s="15"/>
     </row>
-    <row r="33" spans="9:90" ht="15" customHeight="1">
+    <row r="33" spans="1:90" ht="15" customHeight="1">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
@@ -3827,7 +3845,10 @@
       <c r="CK33" s="15"/>
       <c r="CL33" s="15"/>
     </row>
-    <row r="34" spans="9:90" ht="15" customHeight="1">
+    <row r="34" spans="1:90" ht="15" customHeight="1">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
@@ -3915,7 +3936,10 @@
       <c r="CK34" s="15"/>
       <c r="CL34" s="15"/>
     </row>
-    <row r="35" spans="9:90" ht="15" customHeight="1">
+    <row r="35" spans="1:90" ht="15" customHeight="1">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
@@ -3999,7 +4023,10 @@
       <c r="CK35" s="15"/>
       <c r="CL35" s="15"/>
     </row>
-    <row r="36" spans="9:90" ht="15" customHeight="1">
+    <row r="36" spans="1:90" ht="15" customHeight="1">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
@@ -4089,7 +4116,10 @@
       <c r="CK36" s="15"/>
       <c r="CL36" s="15"/>
     </row>
-    <row r="37" spans="9:90" ht="15" customHeight="1">
+    <row r="37" spans="1:90" ht="15" customHeight="1">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>

</xml_diff>